<commit_message>
Primera interfaz (BloqueGeneral y Scoring)
</commit_message>
<xml_diff>
--- a/files/BLOQUE_GENERAL_CCAA.xlsx
+++ b/files/BLOQUE_GENERAL_CCAA.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="BLOQUE_GENERAL_CCAA" sheetId="1" r:id="rId1"/>
+    <sheet name="BLOQUE_GENERAL_CCAA" sheetId="7" r:id="rId1"/>
     <sheet name="CUENTAS_CCAA" sheetId="2" r:id="rId2"/>
     <sheet name="SCORING_CCAA" sheetId="3" r:id="rId3"/>
     <sheet name="DEFINICION_CAMPOS" sheetId="4" r:id="rId4"/>
     <sheet name="Terminología" sheetId="5" r:id="rId5"/>
-    <sheet name="Hoja1" sheetId="6" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15906" uniqueCount="11298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15475" uniqueCount="11298">
   <si>
     <t>CODIGO_CCAA</t>
   </si>
@@ -35001,7 +35000,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -35335,6 +35334,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="42" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="42" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="42" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="41" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="41" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="41" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="41" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="41" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="41" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="23" fillId="40" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="23" fillId="40" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="23" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="37" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -35404,75 +35466,6 @@
     <xf numFmtId="0" fontId="23" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="41" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="41" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="41" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="40" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="40" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="23" fillId="40" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="23" fillId="40" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="23" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="42" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="42" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="42" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="41" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="41" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="41" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -35867,39 +35860,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y63"/>
+  <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Y19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -35978,7 +35945,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>1743</v>
       </c>
@@ -36052,7 +36019,7 @@
         <v>1765</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>1766</v>
       </c>
@@ -36194,7 +36161,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>1801</v>
       </c>
@@ -36271,7 +36238,7 @@
         <v>1819</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>1820</v>
       </c>
@@ -36345,7 +36312,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>1838</v>
       </c>
@@ -36644,7 +36611,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>1909</v>
       </c>
@@ -37289,138 +37256,8 @@
         <v>2053</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -37428,7 +37265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ABU29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="AE1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AG48" sqref="AG48"/>
     </sheetView>
   </sheetViews>
@@ -80874,45 +80711,45 @@
       <c r="KH21"/>
     </row>
     <row r="22" spans="1:749" x14ac:dyDescent="0.25">
-      <c r="Z22">
-        <f>+BLOQUE_GENERAL_CCAA!Y3/CUENTAS_CCAA!FI3</f>
-        <v>1.7500210259389486</v>
+      <c r="Z22" t="e">
+        <f>+#REF!/CUENTAS_CCAA!FI3</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="23" spans="1:749" x14ac:dyDescent="0.25">
-      <c r="Z23">
-        <f>+BLOQUE_GENERAL_CCAA!Y4/CUENTAS_CCAA!FI4</f>
-        <v>1.2020470234368863</v>
+      <c r="Z23" t="e">
+        <f>+#REF!/CUENTAS_CCAA!FI4</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="24" spans="1:749" x14ac:dyDescent="0.25">
-      <c r="Z24">
-        <f>+BLOQUE_GENERAL_CCAA!Y5/CUENTAS_CCAA!FI5</f>
-        <v>2.0047168758909386</v>
+      <c r="Z24" t="e">
+        <f>+#REF!/CUENTAS_CCAA!FI5</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="25" spans="1:749" x14ac:dyDescent="0.25">
-      <c r="Z25">
-        <f>+BLOQUE_GENERAL_CCAA!Y6/CUENTAS_CCAA!FI6</f>
-        <v>0.82202853161645095</v>
+      <c r="Z25" t="e">
+        <f>+#REF!/CUENTAS_CCAA!FI6</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="26" spans="1:749" x14ac:dyDescent="0.25">
-      <c r="Z26">
-        <f>+BLOQUE_GENERAL_CCAA!Y7/CUENTAS_CCAA!FI7</f>
-        <v>1.3487417374136399</v>
+      <c r="Z26" t="e">
+        <f>+#REF!/CUENTAS_CCAA!FI7</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="27" spans="1:749" x14ac:dyDescent="0.25">
-      <c r="Z27">
-        <f>+BLOQUE_GENERAL_CCAA!Y8/CUENTAS_CCAA!FI8</f>
-        <v>1.4382367514458354</v>
+      <c r="Z27" t="e">
+        <f>+#REF!/CUENTAS_CCAA!FI8</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="28" spans="1:749" x14ac:dyDescent="0.25">
-      <c r="Z28">
-        <f>+BLOQUE_GENERAL_CCAA!Y9/CUENTAS_CCAA!FI9</f>
-        <v>2.1748515500003691</v>
+      <c r="Z28" t="e">
+        <f>+#REF!/CUENTAS_CCAA!FI9</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="29" spans="1:749" x14ac:dyDescent="0.25">
@@ -87807,219 +87644,219 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="160">
+      <c r="A7" s="123">
         <v>6</v>
       </c>
       <c r="B7" s="97"/>
       <c r="C7" s="99"/>
-      <c r="D7" s="161" t="s">
+      <c r="D7" s="124" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="160"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="97" t="s">
         <v>174</v>
       </c>
       <c r="C8" s="98" t="s">
         <v>173</v>
       </c>
-      <c r="D8" s="161"/>
+      <c r="D8" s="124"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="160"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="97"/>
       <c r="C9" s="96" t="s">
         <v>146</v>
       </c>
-      <c r="D9" s="161"/>
+      <c r="D9" s="124"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="160"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="95"/>
       <c r="C10" s="94"/>
-      <c r="D10" s="162"/>
+      <c r="D10" s="125"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="163">
+      <c r="A11" s="126">
         <v>7</v>
       </c>
       <c r="B11" s="93"/>
       <c r="C11" s="92"/>
-      <c r="D11" s="164" t="s">
+      <c r="D11" s="128" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="146"/>
+      <c r="A12" s="127"/>
       <c r="B12" s="88"/>
       <c r="C12" s="83" t="s">
         <v>171</v>
       </c>
-      <c r="D12" s="165"/>
+      <c r="D12" s="129"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="146"/>
+      <c r="A13" s="127"/>
       <c r="B13" s="91" t="s">
         <v>170</v>
       </c>
       <c r="C13" s="87" t="s">
         <v>169</v>
       </c>
-      <c r="D13" s="165"/>
+      <c r="D13" s="129"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="146"/>
+      <c r="A14" s="127"/>
       <c r="B14" s="90"/>
       <c r="C14" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="D14" s="165"/>
+      <c r="D14" s="129"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="146"/>
+      <c r="A15" s="127"/>
       <c r="B15" s="88"/>
       <c r="C15" s="87" t="s">
         <v>157</v>
       </c>
-      <c r="D15" s="165"/>
+      <c r="D15" s="129"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="146"/>
+      <c r="A16" s="127"/>
       <c r="B16" s="86"/>
       <c r="C16" s="85"/>
-      <c r="D16" s="166"/>
+      <c r="D16" s="130"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="163">
+      <c r="A17" s="126">
         <v>8</v>
       </c>
       <c r="B17" s="84"/>
       <c r="C17" s="80"/>
-      <c r="D17" s="164" t="s">
+      <c r="D17" s="128" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="146"/>
+      <c r="A18" s="127"/>
       <c r="B18" s="82" t="s">
         <v>166</v>
       </c>
       <c r="C18" s="83" t="s">
         <v>165</v>
       </c>
-      <c r="D18" s="165"/>
+      <c r="D18" s="129"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="146"/>
+      <c r="A19" s="127"/>
       <c r="B19" s="82" t="s">
         <v>164</v>
       </c>
       <c r="C19" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="D19" s="165"/>
+      <c r="D19" s="129"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="146"/>
+      <c r="A20" s="127"/>
       <c r="B20" s="77"/>
       <c r="C20" s="78" t="s">
         <v>162</v>
       </c>
-      <c r="D20" s="165"/>
+      <c r="D20" s="129"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="146"/>
+      <c r="A21" s="127"/>
       <c r="B21" s="77"/>
       <c r="C21" s="76" t="s">
         <v>157</v>
       </c>
-      <c r="D21" s="165"/>
+      <c r="D21" s="129"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="147"/>
+      <c r="A22" s="131"/>
       <c r="B22" s="75"/>
       <c r="C22" s="74"/>
-      <c r="D22" s="166"/>
+      <c r="D22" s="130"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="146">
+      <c r="A23" s="127">
         <v>9</v>
       </c>
       <c r="B23" s="81"/>
       <c r="C23" s="80"/>
-      <c r="D23" s="148" t="s">
+      <c r="D23" s="132" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="146"/>
+      <c r="A24" s="127"/>
       <c r="B24" s="77" t="s">
         <v>160</v>
       </c>
       <c r="C24" s="79" t="s">
         <v>159</v>
       </c>
-      <c r="D24" s="149"/>
+      <c r="D24" s="133"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="146"/>
+      <c r="A25" s="127"/>
       <c r="B25" s="77"/>
       <c r="C25" s="78" t="s">
         <v>158</v>
       </c>
-      <c r="D25" s="149"/>
+      <c r="D25" s="133"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="146"/>
+      <c r="A26" s="127"/>
       <c r="B26" s="77"/>
       <c r="C26" s="76" t="s">
         <v>157</v>
       </c>
-      <c r="D26" s="149"/>
+      <c r="D26" s="133"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="147"/>
+      <c r="A27" s="131"/>
       <c r="B27" s="75"/>
       <c r="C27" s="74"/>
-      <c r="D27" s="150"/>
+      <c r="D27" s="134"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="151">
+      <c r="A28" s="135">
         <v>10</v>
       </c>
       <c r="B28" s="73"/>
       <c r="C28" s="72"/>
-      <c r="D28" s="153" t="s">
+      <c r="D28" s="137" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="36" x14ac:dyDescent="0.25">
-      <c r="A29" s="152"/>
+      <c r="A29" s="136"/>
       <c r="B29" s="70" t="s">
         <v>155</v>
       </c>
       <c r="C29" s="71" t="s">
         <v>154</v>
       </c>
-      <c r="D29" s="154"/>
+      <c r="D29" s="138"/>
     </row>
     <row r="30" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A30" s="152"/>
+      <c r="A30" s="136"/>
       <c r="B30" s="70"/>
       <c r="C30" s="69" t="s">
         <v>153</v>
       </c>
-      <c r="D30" s="154"/>
+      <c r="D30" s="138"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="152"/>
+      <c r="A31" s="136"/>
       <c r="B31" s="68"/>
       <c r="C31" s="67"/>
-      <c r="D31" s="155"/>
+      <c r="D31" s="139"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="156">
+      <c r="A32" s="140">
         <v>11</v>
       </c>
       <c r="B32" s="66" t="s">
@@ -88028,189 +87865,189 @@
       <c r="C32" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="D32" s="158" t="s">
+      <c r="D32" s="142" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="157"/>
+      <c r="A33" s="141"/>
       <c r="B33" s="64"/>
       <c r="C33" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="D33" s="159"/>
+      <c r="D33" s="143"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="134">
+      <c r="A34" s="155">
         <v>12</v>
       </c>
       <c r="B34" s="62"/>
       <c r="C34" s="61"/>
-      <c r="D34" s="137" t="s">
+      <c r="D34" s="158" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="135"/>
+      <c r="A35" s="156"/>
       <c r="B35" s="57" t="s">
         <v>147</v>
       </c>
       <c r="C35" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="D35" s="138"/>
+      <c r="D35" s="159"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="135"/>
+      <c r="A36" s="156"/>
       <c r="B36" s="55"/>
       <c r="C36" s="54" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="138"/>
+      <c r="D36" s="159"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="136"/>
+      <c r="A37" s="157"/>
       <c r="B37" s="53"/>
       <c r="C37" s="60"/>
-      <c r="D37" s="139"/>
+      <c r="D37" s="160"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="140">
+      <c r="A38" s="161">
         <v>13</v>
       </c>
       <c r="B38" s="59"/>
       <c r="C38" s="58"/>
-      <c r="D38" s="137" t="s">
+      <c r="D38" s="158" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="140"/>
+      <c r="A39" s="161"/>
       <c r="B39" s="57" t="s">
         <v>143</v>
       </c>
       <c r="C39" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="D39" s="138"/>
+      <c r="D39" s="159"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="140"/>
+      <c r="A40" s="161"/>
       <c r="B40" s="55"/>
       <c r="C40" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="D40" s="138"/>
+      <c r="D40" s="159"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="141"/>
+      <c r="A41" s="162"/>
       <c r="B41" s="53"/>
       <c r="C41" s="52"/>
-      <c r="D41" s="139"/>
+      <c r="D41" s="160"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="142">
+      <c r="A42" s="163">
         <v>14</v>
       </c>
       <c r="B42" s="51"/>
       <c r="C42" s="50"/>
-      <c r="D42" s="125" t="s">
+      <c r="D42" s="146" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="142"/>
+      <c r="A43" s="163"/>
       <c r="B43" s="49" t="s">
         <v>139</v>
       </c>
       <c r="C43" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="D43" s="144"/>
+      <c r="D43" s="165"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="142"/>
+      <c r="A44" s="163"/>
       <c r="B44" s="42"/>
       <c r="C44" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="D44" s="144"/>
+      <c r="D44" s="165"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="143"/>
+      <c r="A45" s="164"/>
       <c r="B45" s="46"/>
       <c r="C45" s="45"/>
-      <c r="D45" s="145"/>
+      <c r="D45" s="166"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="123">
+      <c r="A46" s="144">
         <v>15</v>
       </c>
       <c r="B46" s="44"/>
       <c r="C46" s="43"/>
-      <c r="D46" s="125" t="s">
+      <c r="D46" s="146" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="123"/>
+      <c r="A47" s="144"/>
       <c r="B47" s="42" t="s">
         <v>136</v>
       </c>
       <c r="C47" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="D47" s="126"/>
+      <c r="D47" s="147"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="123"/>
+      <c r="A48" s="144"/>
       <c r="B48" s="40"/>
       <c r="C48" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="D48" s="126"/>
+      <c r="D48" s="147"/>
     </row>
     <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="124"/>
+      <c r="A49" s="145"/>
       <c r="B49" s="38"/>
       <c r="C49" s="37"/>
-      <c r="D49" s="127"/>
+      <c r="D49" s="148"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="128">
+      <c r="A50" s="149">
         <v>16</v>
       </c>
       <c r="B50" s="36"/>
       <c r="C50" s="35"/>
-      <c r="D50" s="131" t="s">
+      <c r="D50" s="152" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="129"/>
+      <c r="A51" s="150"/>
       <c r="B51" s="33" t="s">
         <v>132</v>
       </c>
       <c r="C51" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="D51" s="132"/>
+      <c r="D51" s="153"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="129"/>
+      <c r="A52" s="150"/>
       <c r="B52" s="33" t="s">
         <v>130</v>
       </c>
       <c r="C52" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="D52" s="132"/>
+      <c r="D52" s="153"/>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="130"/>
+      <c r="A53" s="151"/>
       <c r="B53" s="31"/>
       <c r="C53" s="30"/>
-      <c r="D53" s="133"/>
+      <c r="D53" s="154"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -88866,18 +88703,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="D11:D16"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="D32:D33"/>
     <mergeCell ref="A46:A49"/>
     <mergeCell ref="D46:D49"/>
     <mergeCell ref="A50:A53"/>
@@ -88888,1380 +88713,20 @@
     <mergeCell ref="D38:D41"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="D42:D45"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="D17:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:X19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="118" t="s">
-        <v>312</v>
-      </c>
-      <c r="C1" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="118" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="118" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="118" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="118" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="118" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="118" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="118" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="118" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="118" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="118" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="118" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="118" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="118" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="118" t="s">
-        <v>313</v>
-      </c>
-      <c r="R1" s="118" t="s">
-        <v>189</v>
-      </c>
-      <c r="S1" s="118" t="s">
-        <v>314</v>
-      </c>
-      <c r="T1" s="118" t="s">
-        <v>315</v>
-      </c>
-      <c r="U1" s="118" t="s">
-        <v>316</v>
-      </c>
-      <c r="V1" s="118" t="s">
-        <v>317</v>
-      </c>
-      <c r="W1" s="118" t="s">
-        <v>318</v>
-      </c>
-      <c r="X1" s="118" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="118" t="s">
-        <v>1744</v>
-      </c>
-      <c r="B2" s="120" t="s">
-        <v>1745</v>
-      </c>
-      <c r="C2" s="167" t="s">
-        <v>1746</v>
-      </c>
-      <c r="D2" s="167" t="s">
-        <v>1747</v>
-      </c>
-      <c r="E2" s="167" t="s">
-        <v>1748</v>
-      </c>
-      <c r="F2" s="118" t="s">
-        <v>1749</v>
-      </c>
-      <c r="G2" s="167" t="s">
-        <v>1750</v>
-      </c>
-      <c r="H2" s="118" t="s">
-        <v>1751</v>
-      </c>
-      <c r="I2" s="118" t="s">
-        <v>1752</v>
-      </c>
-      <c r="J2" s="118" t="s">
-        <v>1753</v>
-      </c>
-      <c r="K2" s="118" t="s">
-        <v>1754</v>
-      </c>
-      <c r="L2" s="118" t="s">
-        <v>1755</v>
-      </c>
-      <c r="M2" s="118" t="s">
-        <v>1756</v>
-      </c>
-      <c r="N2" s="118"/>
-      <c r="O2" s="168" t="s">
-        <v>1757</v>
-      </c>
-      <c r="P2" s="168" t="s">
-        <v>1758</v>
-      </c>
-      <c r="Q2" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R2" s="120" t="s">
-        <v>1760</v>
-      </c>
-      <c r="S2" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T2" s="120" t="s">
-        <v>1761</v>
-      </c>
-      <c r="U2" s="120" t="s">
-        <v>1762</v>
-      </c>
-      <c r="V2" s="120" t="s">
-        <v>1763</v>
-      </c>
-      <c r="W2" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X2" s="120" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="118" t="s">
-        <v>1767</v>
-      </c>
-      <c r="B3" s="120" t="s">
-        <v>1768</v>
-      </c>
-      <c r="C3" s="167" t="s">
-        <v>1769</v>
-      </c>
-      <c r="D3" s="167" t="s">
-        <v>1770</v>
-      </c>
-      <c r="E3" s="167" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F3" s="118" t="s">
-        <v>1772</v>
-      </c>
-      <c r="G3" s="118" t="s">
-        <v>1773</v>
-      </c>
-      <c r="H3" s="118" t="s">
-        <v>1774</v>
-      </c>
-      <c r="I3" s="118" t="s">
-        <v>1752</v>
-      </c>
-      <c r="J3" s="118" t="s">
-        <v>1775</v>
-      </c>
-      <c r="K3" s="118" t="s">
-        <v>1776</v>
-      </c>
-      <c r="L3" s="118" t="s">
-        <v>1777</v>
-      </c>
-      <c r="M3" s="118" t="s">
-        <v>1778</v>
-      </c>
-      <c r="N3" s="118"/>
-      <c r="O3" s="168" t="s">
-        <v>1779</v>
-      </c>
-      <c r="P3" s="118"/>
-      <c r="Q3" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R3" s="120" t="s">
-        <v>1780</v>
-      </c>
-      <c r="S3" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T3" s="120" t="s">
-        <v>1781</v>
-      </c>
-      <c r="U3" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V3" s="120" t="s">
-        <v>1782</v>
-      </c>
-      <c r="W3" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X3" s="120" t="s">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="118" t="s">
-        <v>1785</v>
-      </c>
-      <c r="B4" s="120" t="s">
-        <v>1786</v>
-      </c>
-      <c r="C4" s="167" t="s">
-        <v>1787</v>
-      </c>
-      <c r="D4" s="167" t="s">
-        <v>1788</v>
-      </c>
-      <c r="E4" s="167" t="s">
-        <v>1789</v>
-      </c>
-      <c r="F4" s="118" t="s">
-        <v>1790</v>
-      </c>
-      <c r="G4" s="118" t="s">
-        <v>1773</v>
-      </c>
-      <c r="H4" s="118" t="s">
-        <v>1791</v>
-      </c>
-      <c r="I4" s="118" t="s">
-        <v>1792</v>
-      </c>
-      <c r="J4" s="167" t="s">
-        <v>1793</v>
-      </c>
-      <c r="K4" s="118" t="s">
-        <v>1766</v>
-      </c>
-      <c r="L4" s="118" t="s">
-        <v>1794</v>
-      </c>
-      <c r="M4" s="118" t="s">
-        <v>1795</v>
-      </c>
-      <c r="N4" s="118"/>
-      <c r="O4" s="168" t="s">
-        <v>1796</v>
-      </c>
-      <c r="P4" s="118"/>
-      <c r="Q4" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R4" s="120" t="s">
-        <v>1797</v>
-      </c>
-      <c r="S4" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T4" s="120" t="s">
-        <v>1798</v>
-      </c>
-      <c r="U4" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V4" s="120" t="s">
-        <v>1799</v>
-      </c>
-      <c r="W4" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X4" s="120" t="s">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="118" t="s">
-        <v>1802</v>
-      </c>
-      <c r="B5" s="120" t="s">
-        <v>1803</v>
-      </c>
-      <c r="C5" s="167" t="s">
-        <v>1804</v>
-      </c>
-      <c r="D5" s="167" t="s">
-        <v>1805</v>
-      </c>
-      <c r="E5" s="167" t="s">
-        <v>1806</v>
-      </c>
-      <c r="F5" s="118" t="s">
-        <v>1807</v>
-      </c>
-      <c r="G5" s="118" t="s">
-        <v>1773</v>
-      </c>
-      <c r="H5" s="118" t="s">
-        <v>1808</v>
-      </c>
-      <c r="I5" s="118" t="s">
-        <v>1792</v>
-      </c>
-      <c r="J5" s="167" t="s">
-        <v>1809</v>
-      </c>
-      <c r="K5" s="118" t="s">
-        <v>1810</v>
-      </c>
-      <c r="L5" s="118" t="s">
-        <v>1811</v>
-      </c>
-      <c r="M5" s="118" t="s">
-        <v>1812</v>
-      </c>
-      <c r="N5" s="118" t="s">
-        <v>1813</v>
-      </c>
-      <c r="O5" s="168" t="s">
-        <v>1814</v>
-      </c>
-      <c r="P5" s="168" t="s">
-        <v>1815</v>
-      </c>
-      <c r="Q5" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R5" s="120" t="s">
-        <v>1816</v>
-      </c>
-      <c r="S5" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T5" s="120" t="s">
-        <v>1817</v>
-      </c>
-      <c r="U5" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V5" s="120" t="s">
-        <v>1818</v>
-      </c>
-      <c r="W5" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X5" s="120" t="s">
-        <v>1819</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="118" t="s">
-        <v>1821</v>
-      </c>
-      <c r="B6" s="118" t="s">
-        <v>1822</v>
-      </c>
-      <c r="C6" s="167" t="s">
-        <v>1823</v>
-      </c>
-      <c r="D6" s="167" t="s">
-        <v>1824</v>
-      </c>
-      <c r="E6" s="167" t="s">
-        <v>1825</v>
-      </c>
-      <c r="F6" s="118" t="s">
-        <v>1826</v>
-      </c>
-      <c r="G6" s="118" t="s">
-        <v>1773</v>
-      </c>
-      <c r="H6" s="118" t="s">
-        <v>1827</v>
-      </c>
-      <c r="I6" s="118" t="s">
-        <v>1828</v>
-      </c>
-      <c r="J6" s="118" t="s">
-        <v>1829</v>
-      </c>
-      <c r="K6" s="118" t="s">
-        <v>1743</v>
-      </c>
-      <c r="L6" s="118" t="s">
-        <v>1830</v>
-      </c>
-      <c r="M6" s="118" t="s">
-        <v>1831</v>
-      </c>
-      <c r="N6" s="118" t="s">
-        <v>1832</v>
-      </c>
-      <c r="O6" s="168" t="s">
-        <v>1833</v>
-      </c>
-      <c r="P6" s="118"/>
-      <c r="Q6" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R6" s="120" t="s">
-        <v>1834</v>
-      </c>
-      <c r="S6" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T6" s="120" t="s">
-        <v>1835</v>
-      </c>
-      <c r="U6" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V6" s="120" t="s">
-        <v>1836</v>
-      </c>
-      <c r="W6" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X6" s="120" t="s">
-        <v>1837</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="118" t="s">
-        <v>1839</v>
-      </c>
-      <c r="B7" s="120" t="s">
-        <v>1840</v>
-      </c>
-      <c r="C7" s="167" t="s">
-        <v>1841</v>
-      </c>
-      <c r="D7" s="118" t="s">
-        <v>1842</v>
-      </c>
-      <c r="E7" s="118" t="s">
-        <v>1843</v>
-      </c>
-      <c r="F7" s="118" t="s">
-        <v>1844</v>
-      </c>
-      <c r="G7" s="118" t="s">
-        <v>1845</v>
-      </c>
-      <c r="H7" s="118" t="s">
-        <v>1846</v>
-      </c>
-      <c r="I7" s="118" t="s">
-        <v>1792</v>
-      </c>
-      <c r="J7" s="118" t="s">
-        <v>1847</v>
-      </c>
-      <c r="K7" s="118" t="s">
-        <v>1781</v>
-      </c>
-      <c r="L7" s="118" t="s">
-        <v>1848</v>
-      </c>
-      <c r="M7" s="118" t="s">
-        <v>1849</v>
-      </c>
-      <c r="N7" s="118" t="s">
-        <v>1850</v>
-      </c>
-      <c r="O7" s="168" t="s">
-        <v>1851</v>
-      </c>
-      <c r="P7" s="168" t="s">
-        <v>1852</v>
-      </c>
-      <c r="Q7" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R7" s="120" t="s">
-        <v>1853</v>
-      </c>
-      <c r="S7" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T7" s="120" t="s">
-        <v>1854</v>
-      </c>
-      <c r="U7" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V7" s="120" t="s">
-        <v>1855</v>
-      </c>
-      <c r="W7" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X7" s="120" t="s">
-        <v>1856</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="118" t="s">
-        <v>1858</v>
-      </c>
-      <c r="B8" s="120" t="s">
-        <v>1859</v>
-      </c>
-      <c r="C8" s="167" t="s">
-        <v>1860</v>
-      </c>
-      <c r="D8" s="118" t="s">
-        <v>1861</v>
-      </c>
-      <c r="E8" s="167" t="s">
-        <v>1862</v>
-      </c>
-      <c r="F8" s="118" t="s">
-        <v>1863</v>
-      </c>
-      <c r="G8" s="118" t="s">
-        <v>1864</v>
-      </c>
-      <c r="H8" s="118" t="s">
-        <v>1865</v>
-      </c>
-      <c r="I8" s="118" t="s">
-        <v>1828</v>
-      </c>
-      <c r="J8" s="118" t="s">
-        <v>1858</v>
-      </c>
-      <c r="K8" s="118" t="s">
-        <v>1743</v>
-      </c>
-      <c r="L8" s="118" t="s">
-        <v>1866</v>
-      </c>
-      <c r="M8" s="118" t="s">
-        <v>1867</v>
-      </c>
-      <c r="N8" s="118" t="s">
-        <v>1868</v>
-      </c>
-      <c r="O8" s="168" t="s">
-        <v>1869</v>
-      </c>
-      <c r="P8" s="118"/>
-      <c r="Q8" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R8" s="120" t="s">
-        <v>1870</v>
-      </c>
-      <c r="S8" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T8" s="120" t="s">
-        <v>1871</v>
-      </c>
-      <c r="U8" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V8" s="120" t="s">
-        <v>1872</v>
-      </c>
-      <c r="W8" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X8" s="120" t="s">
-        <v>1873</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="118" t="s">
-        <v>1875</v>
-      </c>
-      <c r="B9" s="120" t="s">
-        <v>1876</v>
-      </c>
-      <c r="C9" s="167" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D9" s="167" t="s">
-        <v>1878</v>
-      </c>
-      <c r="E9" s="167" t="s">
-        <v>1879</v>
-      </c>
-      <c r="F9" s="118" t="s">
-        <v>1880</v>
-      </c>
-      <c r="G9" s="118" t="s">
-        <v>1773</v>
-      </c>
-      <c r="H9" s="118" t="s">
-        <v>1881</v>
-      </c>
-      <c r="I9" s="118" t="s">
-        <v>1828</v>
-      </c>
-      <c r="J9" s="118" t="s">
-        <v>1882</v>
-      </c>
-      <c r="K9" s="118" t="s">
-        <v>1820</v>
-      </c>
-      <c r="L9" s="118" t="s">
-        <v>1883</v>
-      </c>
-      <c r="M9" s="118" t="s">
-        <v>1884</v>
-      </c>
-      <c r="N9" s="118" t="s">
-        <v>1885</v>
-      </c>
-      <c r="O9" s="168" t="s">
-        <v>1886</v>
-      </c>
-      <c r="P9" s="118"/>
-      <c r="Q9" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R9" s="120" t="s">
-        <v>1887</v>
-      </c>
-      <c r="S9" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T9" s="120" t="s">
-        <v>1888</v>
-      </c>
-      <c r="U9" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V9" s="120" t="s">
-        <v>1889</v>
-      </c>
-      <c r="W9" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X9" s="120" t="s">
-        <v>1890</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="118" t="s">
-        <v>1892</v>
-      </c>
-      <c r="B10" s="120" t="s">
-        <v>1893</v>
-      </c>
-      <c r="C10" s="118" t="s">
-        <v>1894</v>
-      </c>
-      <c r="D10" s="118" t="s">
-        <v>1895</v>
-      </c>
-      <c r="E10" s="118" t="s">
-        <v>1896</v>
-      </c>
-      <c r="F10" s="118" t="s">
-        <v>1897</v>
-      </c>
-      <c r="G10" s="118" t="s">
-        <v>1898</v>
-      </c>
-      <c r="H10" s="118" t="s">
-        <v>1899</v>
-      </c>
-      <c r="I10" s="118" t="s">
-        <v>1828</v>
-      </c>
-      <c r="J10" s="118" t="s">
-        <v>1900</v>
-      </c>
-      <c r="K10" s="118" t="s">
-        <v>1801</v>
-      </c>
-      <c r="L10" s="118" t="s">
-        <v>1901</v>
-      </c>
-      <c r="M10" s="118" t="s">
-        <v>1902</v>
-      </c>
-      <c r="N10" s="118"/>
-      <c r="O10" s="168" t="s">
-        <v>1903</v>
-      </c>
-      <c r="P10" s="168" t="s">
-        <v>1904</v>
-      </c>
-      <c r="Q10" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R10" s="120" t="s">
-        <v>1905</v>
-      </c>
-      <c r="S10" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T10" s="120" t="s">
-        <v>1906</v>
-      </c>
-      <c r="U10" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V10" s="120" t="s">
-        <v>1907</v>
-      </c>
-      <c r="W10" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X10" s="120" t="s">
-        <v>1908</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="118" t="s">
-        <v>1910</v>
-      </c>
-      <c r="B11" s="120" t="s">
-        <v>1911</v>
-      </c>
-      <c r="C11" s="167" t="s">
-        <v>1912</v>
-      </c>
-      <c r="D11" s="167" t="s">
-        <v>1913</v>
-      </c>
-      <c r="E11" s="167" t="s">
-        <v>1914</v>
-      </c>
-      <c r="F11" s="118" t="s">
-        <v>1915</v>
-      </c>
-      <c r="G11" s="118" t="s">
-        <v>1773</v>
-      </c>
-      <c r="H11" s="118" t="s">
-        <v>1916</v>
-      </c>
-      <c r="I11" s="118" t="s">
-        <v>1792</v>
-      </c>
-      <c r="J11" s="118" t="s">
-        <v>1917</v>
-      </c>
-      <c r="K11" s="118" t="s">
-        <v>1918</v>
-      </c>
-      <c r="L11" s="118" t="s">
-        <v>1919</v>
-      </c>
-      <c r="M11" s="118" t="s">
-        <v>1920</v>
-      </c>
-      <c r="N11" s="118" t="s">
-        <v>1921</v>
-      </c>
-      <c r="O11" s="168" t="s">
-        <v>1922</v>
-      </c>
-      <c r="P11" s="118"/>
-      <c r="Q11" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R11" s="120" t="s">
-        <v>1923</v>
-      </c>
-      <c r="S11" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T11" s="120" t="s">
-        <v>1798</v>
-      </c>
-      <c r="U11" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V11" s="120" t="s">
-        <v>1924</v>
-      </c>
-      <c r="W11" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X11" s="120" t="s">
-        <v>1925</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="118" t="s">
-        <v>1927</v>
-      </c>
-      <c r="B12" s="120" t="s">
-        <v>1928</v>
-      </c>
-      <c r="C12" s="167" t="s">
-        <v>1929</v>
-      </c>
-      <c r="D12" s="118" t="s">
-        <v>1930</v>
-      </c>
-      <c r="E12" s="118" t="s">
-        <v>1931</v>
-      </c>
-      <c r="F12" s="118" t="s">
-        <v>1880</v>
-      </c>
-      <c r="G12" s="118" t="s">
-        <v>1773</v>
-      </c>
-      <c r="H12" s="118" t="s">
-        <v>1932</v>
-      </c>
-      <c r="I12" s="118" t="s">
-        <v>1828</v>
-      </c>
-      <c r="J12" s="118" t="s">
-        <v>1933</v>
-      </c>
-      <c r="K12" s="118" t="s">
-        <v>1754</v>
-      </c>
-      <c r="L12" s="118" t="s">
-        <v>1934</v>
-      </c>
-      <c r="M12" s="118" t="s">
-        <v>1935</v>
-      </c>
-      <c r="N12" s="118" t="s">
-        <v>1936</v>
-      </c>
-      <c r="O12" s="168" t="s">
-        <v>1937</v>
-      </c>
-      <c r="P12" s="168" t="s">
-        <v>1938</v>
-      </c>
-      <c r="Q12" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R12" s="120" t="s">
-        <v>1939</v>
-      </c>
-      <c r="S12" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T12" s="120" t="s">
-        <v>1940</v>
-      </c>
-      <c r="U12" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V12" s="120" t="s">
-        <v>1941</v>
-      </c>
-      <c r="W12" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X12" s="120" t="s">
-        <v>1942</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="118" t="s">
-        <v>1943</v>
-      </c>
-      <c r="B13" s="120" t="s">
-        <v>1944</v>
-      </c>
-      <c r="C13" s="167" t="s">
-        <v>1945</v>
-      </c>
-      <c r="D13" s="118" t="s">
-        <v>1946</v>
-      </c>
-      <c r="E13" s="118" t="s">
-        <v>1947</v>
-      </c>
-      <c r="F13" s="118" t="s">
-        <v>1948</v>
-      </c>
-      <c r="G13" s="118" t="s">
-        <v>1864</v>
-      </c>
-      <c r="H13" s="118" t="s">
-        <v>1949</v>
-      </c>
-      <c r="I13" s="118" t="s">
-        <v>1792</v>
-      </c>
-      <c r="J13" s="118" t="s">
-        <v>1950</v>
-      </c>
-      <c r="K13" s="118" t="s">
-        <v>1754</v>
-      </c>
-      <c r="L13" s="118" t="s">
-        <v>1951</v>
-      </c>
-      <c r="M13" s="118" t="s">
-        <v>1952</v>
-      </c>
-      <c r="N13" s="118" t="s">
-        <v>1953</v>
-      </c>
-      <c r="O13" s="168" t="s">
-        <v>1954</v>
-      </c>
-      <c r="P13" s="168" t="s">
-        <v>1955</v>
-      </c>
-      <c r="Q13" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R13" s="120" t="s">
-        <v>1956</v>
-      </c>
-      <c r="S13" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T13" s="120" t="s">
-        <v>1854</v>
-      </c>
-      <c r="U13" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V13" s="120" t="s">
-        <v>1957</v>
-      </c>
-      <c r="W13" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X13" s="120" t="s">
-        <v>1958</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="118" t="s">
-        <v>1960</v>
-      </c>
-      <c r="B14" s="120" t="s">
-        <v>1961</v>
-      </c>
-      <c r="C14" s="118" t="s">
-        <v>1962</v>
-      </c>
-      <c r="D14" s="167" t="s">
-        <v>1963</v>
-      </c>
-      <c r="E14" s="167" t="s">
-        <v>1964</v>
-      </c>
-      <c r="F14" s="118" t="s">
-        <v>1965</v>
-      </c>
-      <c r="G14" s="118" t="s">
-        <v>1864</v>
-      </c>
-      <c r="H14" s="118" t="s">
-        <v>1966</v>
-      </c>
-      <c r="I14" s="118" t="s">
-        <v>1828</v>
-      </c>
-      <c r="J14" s="118" t="s">
-        <v>1967</v>
-      </c>
-      <c r="K14" s="118" t="s">
-        <v>1857</v>
-      </c>
-      <c r="L14" s="118" t="s">
-        <v>1968</v>
-      </c>
-      <c r="M14" s="118" t="s">
-        <v>1969</v>
-      </c>
-      <c r="N14" s="118" t="s">
-        <v>1970</v>
-      </c>
-      <c r="O14" s="168" t="s">
-        <v>1971</v>
-      </c>
-      <c r="P14" s="168" t="s">
-        <v>1972</v>
-      </c>
-      <c r="Q14" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R14" s="120" t="s">
-        <v>1973</v>
-      </c>
-      <c r="S14" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T14" s="120" t="s">
-        <v>1974</v>
-      </c>
-      <c r="U14" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V14" s="120" t="s">
-        <v>1975</v>
-      </c>
-      <c r="W14" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X14" s="120" t="s">
-        <v>1976</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="118" t="s">
-        <v>1978</v>
-      </c>
-      <c r="B15" s="120" t="s">
-        <v>1979</v>
-      </c>
-      <c r="C15" s="167" t="s">
-        <v>1980</v>
-      </c>
-      <c r="D15" s="118" t="s">
-        <v>1981</v>
-      </c>
-      <c r="E15" s="118" t="s">
-        <v>1982</v>
-      </c>
-      <c r="F15" s="118" t="s">
-        <v>1983</v>
-      </c>
-      <c r="G15" s="118" t="s">
-        <v>1864</v>
-      </c>
-      <c r="H15" s="118" t="s">
-        <v>1984</v>
-      </c>
-      <c r="I15" s="118" t="s">
-        <v>1792</v>
-      </c>
-      <c r="J15" s="118" t="s">
-        <v>1985</v>
-      </c>
-      <c r="K15" s="118" t="s">
-        <v>1754</v>
-      </c>
-      <c r="L15" s="118" t="s">
-        <v>1986</v>
-      </c>
-      <c r="M15" s="118" t="s">
-        <v>1987</v>
-      </c>
-      <c r="N15" s="118" t="s">
-        <v>1988</v>
-      </c>
-      <c r="O15" s="168" t="s">
-        <v>1989</v>
-      </c>
-      <c r="P15" s="169" t="s">
-        <v>1990</v>
-      </c>
-      <c r="Q15" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R15" s="120" t="s">
-        <v>1991</v>
-      </c>
-      <c r="S15" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T15" s="120" t="s">
-        <v>1835</v>
-      </c>
-      <c r="U15" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V15" s="120" t="s">
-        <v>1992</v>
-      </c>
-      <c r="W15" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X15" s="120" t="s">
-        <v>1993</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="118" t="s">
-        <v>1995</v>
-      </c>
-      <c r="B16" s="120" t="s">
-        <v>1996</v>
-      </c>
-      <c r="C16" s="167" t="s">
-        <v>1997</v>
-      </c>
-      <c r="D16" s="167" t="s">
-        <v>1998</v>
-      </c>
-      <c r="E16" s="167" t="s">
-        <v>1999</v>
-      </c>
-      <c r="F16" s="118" t="s">
-        <v>2000</v>
-      </c>
-      <c r="G16" s="118" t="s">
-        <v>1773</v>
-      </c>
-      <c r="H16" s="118" t="s">
-        <v>2001</v>
-      </c>
-      <c r="I16" s="118" t="s">
-        <v>2002</v>
-      </c>
-      <c r="J16" s="118" t="s">
-        <v>2003</v>
-      </c>
-      <c r="K16" s="118" t="s">
-        <v>1743</v>
-      </c>
-      <c r="L16" s="118" t="s">
-        <v>2004</v>
-      </c>
-      <c r="M16" s="118" t="s">
-        <v>2005</v>
-      </c>
-      <c r="N16" s="118"/>
-      <c r="O16" s="168" t="s">
-        <v>2006</v>
-      </c>
-      <c r="P16" s="168" t="s">
-        <v>2007</v>
-      </c>
-      <c r="Q16" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R16" s="120" t="s">
-        <v>2008</v>
-      </c>
-      <c r="S16" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T16" s="120" t="s">
-        <v>2009</v>
-      </c>
-      <c r="U16" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V16" s="120" t="s">
-        <v>2010</v>
-      </c>
-      <c r="W16" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X16" s="120" t="s">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="118" t="s">
-        <v>2013</v>
-      </c>
-      <c r="B17" s="120" t="s">
-        <v>2014</v>
-      </c>
-      <c r="C17" s="167" t="s">
-        <v>2015</v>
-      </c>
-      <c r="D17" s="118" t="s">
-        <v>2016</v>
-      </c>
-      <c r="E17" s="118" t="s">
-        <v>2017</v>
-      </c>
-      <c r="F17" s="118" t="s">
-        <v>2018</v>
-      </c>
-      <c r="G17" s="118" t="s">
-        <v>2019</v>
-      </c>
-      <c r="H17" s="118" t="s">
-        <v>2020</v>
-      </c>
-      <c r="I17" s="118" t="s">
-        <v>1792</v>
-      </c>
-      <c r="J17" s="167" t="s">
-        <v>2021</v>
-      </c>
-      <c r="K17" s="118" t="s">
-        <v>1743</v>
-      </c>
-      <c r="L17" s="118" t="s">
-        <v>2022</v>
-      </c>
-      <c r="M17" s="118" t="s">
-        <v>2023</v>
-      </c>
-      <c r="N17" s="118" t="s">
-        <v>2024</v>
-      </c>
-      <c r="O17" s="168" t="s">
-        <v>2025</v>
-      </c>
-      <c r="P17" s="168" t="s">
-        <v>2026</v>
-      </c>
-      <c r="Q17" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R17" s="120" t="s">
-        <v>2027</v>
-      </c>
-      <c r="S17" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T17" s="120" t="s">
-        <v>2028</v>
-      </c>
-      <c r="U17" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V17" s="120" t="s">
-        <v>2029</v>
-      </c>
-      <c r="W17" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X17" s="120" t="s">
-        <v>2030</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="118" t="s">
-        <v>2031</v>
-      </c>
-      <c r="B18" s="120" t="s">
-        <v>2032</v>
-      </c>
-      <c r="C18" s="167" t="s">
-        <v>2033</v>
-      </c>
-      <c r="D18" s="167" t="s">
-        <v>2034</v>
-      </c>
-      <c r="E18" s="167" t="s">
-        <v>1789</v>
-      </c>
-      <c r="F18" s="118" t="s">
-        <v>2035</v>
-      </c>
-      <c r="G18" s="118" t="s">
-        <v>1773</v>
-      </c>
-      <c r="H18" s="118" t="s">
-        <v>2036</v>
-      </c>
-      <c r="I18" s="118" t="s">
-        <v>1792</v>
-      </c>
-      <c r="J18" s="118" t="s">
-        <v>2037</v>
-      </c>
-      <c r="K18" s="118" t="s">
-        <v>1784</v>
-      </c>
-      <c r="L18" s="118" t="s">
-        <v>2038</v>
-      </c>
-      <c r="M18" s="118" t="s">
-        <v>2039</v>
-      </c>
-      <c r="N18" s="118" t="s">
-        <v>2040</v>
-      </c>
-      <c r="O18" s="168" t="s">
-        <v>2041</v>
-      </c>
-      <c r="P18" s="168" t="s">
-        <v>2042</v>
-      </c>
-      <c r="Q18" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R18" s="120" t="s">
-        <v>2043</v>
-      </c>
-      <c r="S18" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T18" s="120" t="s">
-        <v>2044</v>
-      </c>
-      <c r="U18" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V18" s="120" t="s">
-        <v>2045</v>
-      </c>
-      <c r="W18" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X18" s="120" t="s">
-        <v>2046</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="118" t="s">
-        <v>2047</v>
-      </c>
-      <c r="B19" s="118" t="s">
-        <v>2048</v>
-      </c>
-      <c r="C19" s="118"/>
-      <c r="D19" s="118"/>
-      <c r="E19" s="118"/>
-      <c r="F19" s="118"/>
-      <c r="G19" s="118"/>
-      <c r="H19" s="118"/>
-      <c r="I19" s="118"/>
-      <c r="J19" s="118"/>
-      <c r="K19" s="118"/>
-      <c r="L19" s="118"/>
-      <c r="M19" s="118"/>
-      <c r="N19" s="118"/>
-      <c r="O19" s="118"/>
-      <c r="P19" s="118"/>
-      <c r="Q19" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="R19" s="120" t="s">
-        <v>2049</v>
-      </c>
-      <c r="S19" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="T19" s="120" t="s">
-        <v>2050</v>
-      </c>
-      <c r="U19" s="120" t="s">
-        <v>1759</v>
-      </c>
-      <c r="V19" s="120" t="s">
-        <v>2051</v>
-      </c>
-      <c r="W19" s="170" t="s">
-        <v>2052</v>
-      </c>
-      <c r="X19" s="170" t="s">
-        <v>2053</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>